<commit_message>
Separate Sidebars as per roles
</commit_message>
<xml_diff>
--- a/Docs/Logics.xlsx
+++ b/Docs/Logics.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikhil\source\repos\Qeros\HRMS\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D553F113-1DB6-44EC-BDD7-43910777CB0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E86E6090-A259-41E8-AEEF-630E682F248B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Roles" sheetId="1" r:id="rId1"/>
+    <sheet name="Pages" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="19">
   <si>
     <t>Dashboard</t>
   </si>
@@ -79,6 +80,9 @@
   </si>
   <si>
     <t>Yes [ByPassToken]</t>
+  </si>
+  <si>
+    <t>ecommerce-page/order-details</t>
   </si>
 </sst>
 </file>
@@ -408,7 +412,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
@@ -613,4 +617,27 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30F50B59-97DA-438E-B05E-00CBEA7C4EFF}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="40.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added Separate Dashboard Sidebars
</commit_message>
<xml_diff>
--- a/Docs/Logics.xlsx
+++ b/Docs/Logics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikhil\source\repos\Qeros\HRMS\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E86E6090-A259-41E8-AEEF-630E682F248B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB7DFEB5-4E66-468F-A4FA-6AE0EC24AEAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Roles" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="20">
   <si>
     <t>Dashboard</t>
   </si>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t>ecommerce-page/order-details</t>
+  </si>
+  <si>
+    <t>Yes [ByPassToken]-Access when Status Complete</t>
   </si>
 </sst>
 </file>
@@ -412,15 +415,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.21875" customWidth="1"/>
     <col min="2" max="2" width="16.5546875" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" customWidth="1"/>
+    <col min="3" max="3" width="26.21875" customWidth="1"/>
     <col min="4" max="4" width="18.33203125" customWidth="1"/>
     <col min="5" max="5" width="19.88671875" customWidth="1"/>
     <col min="6" max="6" width="19.21875" customWidth="1"/>
@@ -601,7 +604,7 @@
         <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D11" t="s">
         <v>6</v>
@@ -610,7 +613,7 @@
         <v>7</v>
       </c>
       <c r="F11" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -623,7 +626,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30F50B59-97DA-438E-B05E-00CBEA7C4EFF}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Finalized Admin Sidebar Menu Items
</commit_message>
<xml_diff>
--- a/Docs/Logics.xlsx
+++ b/Docs/Logics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikhil\source\repos\Qeros\HRMS\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB7DFEB5-4E66-468F-A4FA-6AE0EC24AEAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA929A77-7D25-47ED-A020-8003C9CD8954}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -416,17 +416,17 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.21875" customWidth="1"/>
     <col min="2" max="2" width="16.5546875" customWidth="1"/>
-    <col min="3" max="3" width="26.21875" customWidth="1"/>
+    <col min="3" max="3" width="41.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.33203125" customWidth="1"/>
     <col min="5" max="5" width="19.88671875" customWidth="1"/>
-    <col min="6" max="6" width="19.21875" customWidth="1"/>
+    <col min="6" max="6" width="40.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">

</xml_diff>